<commit_message>
Update Power_ThermalGen to v0.0.4r
(de)comYear to Year(De)Com
Excl. to excl
Corrections in human readable name
</commit_message>
<xml_diff>
--- a/examples/Power_ThermalGen.xlsx
+++ b/examples/Power_ThermalGen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3339901A-7C78-4648-BF76-C49952727E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B93842-68ED-4B45-AB2A-8ECA6447C59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41895" yWindow="-19440" windowWidth="21600" windowHeight="12645" tabRatio="733" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="105" r:id="rId1"/>
@@ -243,7 +243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="128">
   <si>
     <t>[MW]</t>
   </si>
@@ -410,9 +410,6 @@
     <t>lat</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>[h]</t>
   </si>
   <si>
@@ -617,7 +614,19 @@
     <t>Equivalent forced outage rate of the generator</t>
   </si>
   <si>
-    <t>v0.0.3</t>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>lon</t>
+  </si>
+  <si>
+    <t>Commission Year</t>
+  </si>
+  <si>
+    <t>Decommission Year</t>
   </si>
 </sst>
 </file>
@@ -1241,27 +1250,27 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>12</v>
@@ -1279,10 +1288,10 @@
         <v>8</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>15</v>
@@ -1297,16 +1306,16 @@
         <v>2</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>6</v>
@@ -1324,39 +1333,39 @@
         <v>19</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="AD3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE3" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>12</v>
@@ -1374,10 +1383,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>15</v>
@@ -1392,16 +1401,16 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>6</v>
@@ -1428,214 +1437,214 @@
         <v>54</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="AD4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE4" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="AE4" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="U5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="W5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AD5" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="AE5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
@@ -1653,10 +1662,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>17</v>
@@ -1671,19 +1680,19 @@
         <v>1</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>11</v>
@@ -1692,28 +1701,28 @@
         <v>41</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE7" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="AE7" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -1799,10 +1808,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE8" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE8" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -1888,10 +1897,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE9" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE9" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -1977,10 +1986,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE10" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE10" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -2066,10 +2075,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE11" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE11" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -2155,10 +2164,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE12" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE12" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -2244,10 +2253,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE13" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE13" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -2333,10 +2342,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE14" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE14" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -2422,10 +2431,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD15" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE15" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -2511,15 +2520,15 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD16" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE16" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
@@ -2602,10 +2611,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE17" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE17" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -2691,10 +2700,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE18" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE18" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -2780,10 +2789,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE19" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE19" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -2869,10 +2878,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE20" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE20" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -2958,10 +2967,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE21" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE21" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -3047,10 +3056,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE22" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE22" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -3136,10 +3145,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE23" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE23" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -3225,10 +3234,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD24" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE24" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE24" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -3314,10 +3323,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD25" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE25" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -3403,10 +3412,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD26" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE26" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -3492,10 +3501,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD27" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE27" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE27" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" spans="15:17" x14ac:dyDescent="0.25">
@@ -3632,27 +3641,27 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>12</v>
@@ -3670,10 +3679,10 @@
         <v>8</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>15</v>
@@ -3688,16 +3697,16 @@
         <v>2</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>3</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U3" s="6" t="s">
         <v>6</v>
@@ -3715,39 +3724,39 @@
         <v>19</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>52</v>
+        <v>126</v>
       </c>
       <c r="AA3" s="6" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
       <c r="AB3" s="6" t="s">
-        <v>54</v>
+        <v>118</v>
       </c>
       <c r="AC3" s="6" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
       <c r="AD3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE3" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>59</v>
+        <v>124</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>12</v>
@@ -3765,10 +3774,10 @@
         <v>8</v>
       </c>
       <c r="K4" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>15</v>
@@ -3783,16 +3792,16 @@
         <v>2</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>6</v>
@@ -3819,214 +3828,214 @@
         <v>54</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="AD4" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="AE4" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="AE4" s="7" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:31" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="E5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="G5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="K5" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="L5" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="N5" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="Q5" s="9" t="s">
+      <c r="R5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="T5" s="9" t="s">
+      <c r="U5" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="V5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="U5" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="W5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="X5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="Y5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="AA5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AB5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AD5" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AD5" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="AE5" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="R6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Y6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AC6" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AD6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE6" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
@@ -4044,10 +4053,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>17</v>
@@ -4062,19 +4071,19 @@
         <v>1</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>11</v>
@@ -4083,28 +4092,28 @@
         <v>41</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AB7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AD7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE7" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="AE7" s="4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -4190,10 +4199,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD8" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE8" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE8" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -4279,10 +4288,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE9" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE9" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -4368,10 +4377,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE10" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE10" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -4457,10 +4466,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD11" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE11" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE11" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -4546,10 +4555,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD12" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE12" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE12" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -4635,10 +4644,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD13" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE13" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE13" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -4724,10 +4733,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD14" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE14" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE14" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -4813,10 +4822,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD15" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE15" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -4902,15 +4911,15 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD16" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE16" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
@@ -4993,10 +5002,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD17" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE17" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE17" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -5082,10 +5091,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD18" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE18" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE18" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -5171,10 +5180,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD19" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE19" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE19" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -5260,10 +5269,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD20" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE20" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE20" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -5349,10 +5358,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD21" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE21" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE21" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -5438,10 +5447,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD22" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE22" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE22" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -5527,10 +5536,10 @@
         <v>14.479570000000001</v>
       </c>
       <c r="AD23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE23" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE23" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -5616,10 +5625,10 @@
         <v>9.9000199999999996</v>
       </c>
       <c r="AD24" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE24" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE24" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -5705,10 +5714,10 @@
         <v>9.9157949999999992</v>
       </c>
       <c r="AD25" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE25" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -5794,10 +5803,10 @@
         <v>12.818199999999999</v>
       </c>
       <c r="AD26" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE26" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -5883,10 +5892,10 @@
         <v>13.746700000000001</v>
       </c>
       <c r="AD27" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE27" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AE27" s="16" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="33" spans="19:19" x14ac:dyDescent="0.25">
@@ -5903,21 +5912,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -6063,31 +6057,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6103,4 +6088,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>